<commit_message>
Added database setup in .sql file and updated table translation some
</commit_message>
<xml_diff>
--- a/diagrams/Table Translation.xlsx
+++ b/diagrams/Table Translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
   <si>
     <t xml:space="preserve">Users</t>
   </si>
@@ -73,6 +73,9 @@
     <t xml:space="preserve">SSN</t>
   </si>
   <si>
+    <t xml:space="preserve">Varchar(9)</t>
+  </si>
+  <si>
     <t xml:space="preserve">NOT NULL     Len(9)</t>
   </si>
   <si>
@@ -101,6 +104,24 @@
   </si>
   <si>
     <t xml:space="preserve">FK (Applications.appli_num)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zip_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varchar(100) </t>
   </si>
 </sst>
 </file>
@@ -220,10 +241,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:G19"/>
+  <dimension ref="A3:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,30 +383,30 @@
         <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>6</v>
@@ -393,24 +414,24 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,10 +462,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>6</v>
@@ -461,7 +482,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>9</v>
@@ -474,6 +495,15 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="E19" s="0" t="s">
         <v>12</v>
       </c>
@@ -481,6 +511,50 @@
         <v>13</v>
       </c>
       <c r="G19" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
forgot to save the table translation
</commit_message>
<xml_diff>
--- a/diagrams/Table Translation.xlsx
+++ b/diagrams/Table Translation.xlsx
@@ -106,7 +106,7 @@
     <t xml:space="preserve">FK (Applications.appli_num)</t>
   </si>
   <si>
-    <t xml:space="preserve">street add</t>
+    <t xml:space="preserve">street addr</t>
   </si>
   <si>
     <t xml:space="preserve">city</t>
@@ -244,7 +244,7 @@
   <dimension ref="A3:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
I guess I didn't commit the signup page
</commit_message>
<xml_diff>
--- a/diagrams/Table Translation.xlsx
+++ b/diagrams/Table Translation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
   <si>
     <t xml:space="preserve">Users</t>
   </si>
@@ -116,12 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve">zip_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varchar(100) </t>
   </si>
 </sst>
 </file>
@@ -136,6 +130,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,6 +152,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -244,10 +240,10 @@
   <dimension ref="A3:G23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
@@ -282,116 +278,116 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="0" t="s">
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -399,38 +395,38 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -455,108 +451,102 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="F17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="0" t="s">
+      <c r="F18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="0" t="s">
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>11</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>